<commit_message>
Changed album data collection method for easy line-up with Tony Award dataset and track data
</commit_message>
<xml_diff>
--- a/Data/Tony_Winner_Spreadsheet.xlsx
+++ b/Data/Tony_Winner_Spreadsheet.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morganhogenmiller/repos/Tony_Win_Music_Scraping/scripts/album_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morganhogenmiller/repos/Tony_Win_Music_Scraping/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="11200" yWindow="460" windowWidth="10000" windowHeight="11140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,9 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Tony Winner</t>
   </si>
   <si>
@@ -41,57 +38,15 @@
     <t>South Pacific</t>
   </si>
   <si>
-    <t>The Pajama Game</t>
-  </si>
-  <si>
-    <t>The Sound of Music</t>
-  </si>
-  <si>
-    <t>Fiddler on the Roof</t>
-  </si>
-  <si>
     <t>Applause</t>
   </si>
   <si>
     <t>The Wiz</t>
   </si>
   <si>
-    <t>Evita</t>
-  </si>
-  <si>
-    <t>Big River</t>
-  </si>
-  <si>
-    <t>City of Angels</t>
-  </si>
-  <si>
-    <t>Sunset Boulevard</t>
-  </si>
-  <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>Spamalot</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Fun Home</t>
-  </si>
-  <si>
-    <t>Hamilton</t>
-  </si>
-  <si>
-    <t>Dear Evan Hansen</t>
-  </si>
-  <si>
-    <t>Hadestown</t>
-  </si>
-  <si>
-    <t>The Band's Visit</t>
-  </si>
-  <si>
     <t>spotify:album:2WQ4A0NReQExTbR70sFLtN</t>
   </si>
   <si>
@@ -144,19 +99,69 @@
   </si>
   <si>
     <t>spotify:album:1J1yxODbNlqKbwRqJxYJUP</t>
+  </si>
+  <si>
+    <t>Monty Python's Spamalot</t>
+  </si>
+  <si>
+    <t>Tony Win Year</t>
+  </si>
+  <si>
+    <t>The Pajama Game (Original Broadway Cast Recording)</t>
+  </si>
+  <si>
+    <t>The Sound of Music - Original Soundtrack Recording</t>
+  </si>
+  <si>
+    <t>Fiddler on the Roof (Original Broadway Cast Recording)</t>
+  </si>
+  <si>
+    <t>Evita (Original London Cast Recording)</t>
+  </si>
+  <si>
+    <t>Big River: The Adventures Of Huckleberry Finn</t>
+  </si>
+  <si>
+    <t>City of Angels (Original Broadway Cast Recording)</t>
+  </si>
+  <si>
+    <t>Sunset Boulevard (Original Broadway Cast)</t>
+  </si>
+  <si>
+    <t>Memphis: A New Musical [Original Cast Recording]</t>
+  </si>
+  <si>
+    <t>Fun Home (A New Broadway Musical)</t>
+  </si>
+  <si>
+    <t>Hamilton (Original Broadway Cast Recording)</t>
+  </si>
+  <si>
+    <t>Dear Evan Hansen (Original Broadway Cast Recording)</t>
+  </si>
+  <si>
+    <t>The Band's Visit (Original Broadway Cast Recording)</t>
+  </si>
+  <si>
+    <t>Hadestown (Original Broadway Cast Recording)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,8 +184,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,24 +468,25 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -486,43 +494,43 @@
         <v>1950</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1955</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1960</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1965</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -530,10 +538,10 @@
         <v>1970</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -541,54 +549,54 @@
         <v>1975</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1980</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1985</v>
       </c>
-      <c r="B9" t="s">
-        <v>10</v>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1990</v>
       </c>
-      <c r="B10" t="s">
-        <v>11</v>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1995</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -596,10 +604,10 @@
         <v>2000</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -607,76 +615,76 @@
         <v>2005</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2010</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2015</v>
       </c>
-      <c r="B15" t="s">
-        <v>16</v>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2016</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2017</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2018</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2019</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>